<commit_message>
found chromatic number on monstergraph B3-05 (bipartite)
</commit_message>
<xml_diff>
--- a/someResults.xlsx
+++ b/someResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alain\Desktop\project1-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8652F68B-E6A2-4DB8-934B-98365567F176}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C548006-3DF8-4E59-84D2-F6F8F4010F37}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5568" xr2:uid="{BBF5B598-23F2-4CAF-8950-11568DE92F9C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17254" windowHeight="5571" xr2:uid="{BBF5B598-23F2-4CAF-8950-11568DE92F9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="43">
   <si>
     <t>goal</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>Graph 20</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -531,16 +528,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79E6403-583E-4F38-A99A-D9FFC217D789}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +545,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -556,7 +553,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -564,7 +561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -572,7 +569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -580,7 +577,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -588,7 +585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -596,7 +593,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -604,7 +601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -612,7 +609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -620,7 +617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -628,7 +625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -636,7 +633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -644,7 +641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -652,7 +649,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -660,7 +657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -668,7 +665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -676,7 +673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -684,7 +681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -692,7 +689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -700,7 +697,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -708,12 +705,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -721,7 +718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -729,7 +726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -737,7 +734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -745,15 +742,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -761,7 +758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -769,7 +766,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -777,7 +774,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -785,7 +782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -793,7 +790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -801,7 +798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
@@ -809,7 +806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -817,7 +814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
@@ -825,7 +822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -833,7 +830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
@@ -841,7 +838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -849,7 +846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
@@ -857,7 +854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
@@ -865,7 +862,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
some tweaking on the odd cycle finder
</commit_message>
<xml_diff>
--- a/someResults.xlsx
+++ b/someResults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alain\Desktop\project1-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C548006-3DF8-4E59-84D2-F6F8F4010F37}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7BD48E-1ECE-4C3B-9C1A-7D205569CDEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17254" windowHeight="5571" xr2:uid="{BBF5B598-23F2-4CAF-8950-11568DE92F9C}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>goal</t>
   </si>
@@ -160,6 +161,18 @@
   </si>
   <si>
     <t>Graph 20</t>
+  </si>
+  <si>
+    <t>max clique</t>
+  </si>
+  <si>
+    <t>odd cycle</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -526,26 +539,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79E6403-583E-4F38-A99A-D9FFC217D789}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I38" sqref="I35:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -553,7 +573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -561,7 +581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -569,7 +589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -577,7 +597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -585,7 +605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -593,7 +613,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -601,7 +621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -609,7 +629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -617,7 +637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -625,7 +645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -633,7 +653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -641,7 +661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -649,7 +669,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -657,7 +677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -665,7 +685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -673,7 +693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -681,7 +701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -689,7 +709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -697,7 +717,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -705,169 +725,289 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E23" s="2">
+        <v>3</v>
+      </c>
+      <c r="G23" s="2">
+        <v>3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E24" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="I24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="I25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E26" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="I26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G27" s="2">
+        <v>2</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E28" s="2">
+        <v>3</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3</v>
+      </c>
+      <c r="I28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E29" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G29">
+        <v>8</v>
+      </c>
+      <c r="I29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E30" s="3">
         <v>98</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G30">
+        <v>6</v>
+      </c>
+      <c r="I30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E31" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="I31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E32" s="2">
+        <v>3</v>
+      </c>
+      <c r="G32" s="2">
+        <v>3</v>
+      </c>
+      <c r="I32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E33" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="I33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G34" s="2">
+        <v>2</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E35" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G35">
+        <v>7</v>
+      </c>
+      <c r="I35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E36" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E37" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="I37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E38" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="I38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E39" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G39">
+        <v>6</v>
+      </c>
+      <c r="I39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E40" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G40">
+        <v>6</v>
+      </c>
+      <c r="I40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E41" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G41">
+        <v>6</v>
+      </c>
+      <c r="I41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E42" s="3">
         <v>9</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+      <c r="I42" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some more results
</commit_message>
<xml_diff>
--- a/someResults.xlsx
+++ b/someResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alain\Desktop\project1-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E049F71E-310F-4172-A70E-A6B82DAC6793}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E75B930-AD22-4E62-BC6D-767EF5B5FE1E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17254" windowHeight="5571" xr2:uid="{BBF5B598-23F2-4CAF-8950-11568DE92F9C}"/>
   </bookViews>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
-  <si>
-    <t>goal</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>Graph 01        5</t>
   </si>
@@ -97,9 +94,6 @@
     <t>Graph 20        4</t>
   </si>
   <si>
-    <t>Best DSATUR</t>
-  </si>
-  <si>
     <t xml:space="preserve">block3 </t>
   </si>
   <si>
@@ -173,6 +167,24 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>&lt;- finished</t>
+  </si>
+  <si>
+    <t>&lt;-finished</t>
+  </si>
+  <si>
+    <t>Geller LB</t>
+  </si>
+  <si>
+    <t>Best DSAT</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>size</t>
   </si>
 </sst>
 </file>
@@ -194,7 +206,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +216,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,11 +250,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -539,214 +572,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79E6403-583E-4F38-A99A-D9FFC217D789}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I38" sqref="I35:I38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="1" max="1" width="29.69140625" customWidth="1"/>
+    <col min="2" max="2" width="6.15234375" customWidth="1"/>
+    <col min="5" max="5" width="9.4609375" customWidth="1"/>
+    <col min="6" max="6" width="2.4609375" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="9.84375" customWidth="1"/>
+    <col min="10" max="10" width="2.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
       <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="E2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G10" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G16" s="5">
+        <v>3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G17" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="G18" s="5">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E18" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E19" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>212</v>
+      </c>
+      <c r="C23">
+        <v>252</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3</v>
+      </c>
+      <c r="G23" s="2">
+        <v>3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23">
+        <f>(SUMSQ(B23)/(SUMSQ(B23)-2*C23))</f>
+        <v>1.0113411341134113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="2">
-        <v>3</v>
-      </c>
-      <c r="G23" s="2">
-        <v>3</v>
-      </c>
-      <c r="I23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
+      <c r="B24">
+        <v>456</v>
+      </c>
+      <c r="C24">
+        <v>1028</v>
       </c>
       <c r="E24" s="3">
         <v>4</v>
@@ -755,12 +881,22 @@
         <v>3</v>
       </c>
       <c r="I24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K24">
+        <f t="shared" ref="K24:K42" si="0">(SUMSQ(B24)/(SUMSQ(B24)-2*C24))</f>
+        <v>1.0099863998445697</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>218</v>
+      </c>
+      <c r="C25">
+        <v>1267</v>
       </c>
       <c r="E25" s="3">
         <v>7</v>
@@ -769,12 +905,22 @@
         <v>4</v>
       </c>
       <c r="I25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>1.0563236274727716</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>107</v>
+      </c>
+      <c r="C26">
+        <v>516</v>
       </c>
       <c r="E26" s="3">
         <v>5</v>
@@ -783,12 +929,22 @@
         <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>1.0990688297974465</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>4007</v>
+      </c>
+      <c r="C27">
+        <v>1198933</v>
       </c>
       <c r="E27" s="2">
         <v>2</v>
@@ -797,12 +953,22 @@
         <v>2</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>1.1755625913051539</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>529</v>
+      </c>
+      <c r="C28">
+        <v>271</v>
       </c>
       <c r="E28" s="2">
         <v>3</v>
@@ -811,12 +977,22 @@
         <v>3</v>
       </c>
       <c r="I28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>1.0019405726479507</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>43</v>
+      </c>
+      <c r="C29">
+        <v>529</v>
       </c>
       <c r="E29" s="3">
         <v>12</v>
@@ -825,12 +1001,22 @@
         <v>8</v>
       </c>
       <c r="I29" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>2.3375474083438683</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>107</v>
+      </c>
+      <c r="C30">
+        <v>4955</v>
       </c>
       <c r="E30" s="3">
         <v>98</v>
@@ -839,12 +1025,22 @@
         <v>6</v>
       </c>
       <c r="I30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" si="0"/>
+        <v>7.4392462638076671</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>206</v>
+      </c>
+      <c r="C31">
+        <v>961</v>
       </c>
       <c r="E31" s="3">
         <v>5</v>
@@ -853,12 +1049,22 @@
         <v>3</v>
       </c>
       <c r="I31" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>1.0474403909759589</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>166</v>
+      </c>
+      <c r="C32">
+        <v>197</v>
       </c>
       <c r="E32" s="2">
         <v>3</v>
@@ -867,12 +1073,22 @@
         <v>3</v>
       </c>
       <c r="I32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>1.0145055592371697</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>164</v>
+      </c>
+      <c r="C33">
+        <v>889</v>
       </c>
       <c r="E33" s="3">
         <v>15</v>
@@ -881,12 +1097,22 @@
         <v>5</v>
       </c>
       <c r="I33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>1.070785890596385</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>744</v>
+      </c>
+      <c r="C34">
+        <v>744</v>
       </c>
       <c r="E34" s="2">
         <v>2</v>
@@ -895,12 +1121,22 @@
         <v>2</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>1.0026954177897573</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>85</v>
+      </c>
+      <c r="C35">
+        <v>1060</v>
       </c>
       <c r="E35" s="3">
         <v>13</v>
@@ -909,12 +1145,22 @@
         <v>7</v>
       </c>
       <c r="I35" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>1.4152791380999021</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>907</v>
+      </c>
+      <c r="C36">
+        <v>1808</v>
       </c>
       <c r="E36" s="3">
         <v>4</v>
@@ -923,12 +1169,22 @@
         <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>1.0044149625228775</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>215</v>
+      </c>
+      <c r="C37">
+        <v>1642</v>
       </c>
       <c r="E37" s="3">
         <v>9</v>
@@ -937,12 +1193,22 @@
         <v>5</v>
       </c>
       <c r="I37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>1.0764770266179176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>164</v>
+      </c>
+      <c r="C38">
+        <v>323</v>
       </c>
       <c r="E38" s="3">
         <v>4</v>
@@ -951,12 +1217,22 @@
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="0"/>
+        <v>1.0246095238095239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>106</v>
+      </c>
+      <c r="C39">
+        <v>96</v>
       </c>
       <c r="E39" s="3">
         <v>8</v>
@@ -965,12 +1241,22 @@
         <v>6</v>
       </c>
       <c r="I39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>1.0173850054328142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>131</v>
+      </c>
+      <c r="C40">
+        <v>1116</v>
       </c>
       <c r="E40" s="3">
         <v>10</v>
@@ -979,12 +1265,22 @@
         <v>6</v>
       </c>
       <c r="I40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="0"/>
+        <v>1.1495076696362785</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>143</v>
+      </c>
+      <c r="C41">
+        <v>498</v>
       </c>
       <c r="E41" s="3">
         <v>11</v>
@@ -993,12 +1289,22 @@
         <v>6</v>
       </c>
       <c r="I41" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="0"/>
+        <v>1.051200328998098</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>387</v>
+      </c>
+      <c r="C42">
+        <v>2502</v>
       </c>
       <c r="E42" s="3">
         <v>9</v>
@@ -1007,7 +1313,11 @@
         <v>5</v>
       </c>
       <c r="I42" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>1.0345663661796705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished simple backtracking algorithm
</commit_message>
<xml_diff>
--- a/someResults.xlsx
+++ b/someResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alain\Desktop\project1-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DB29109-C9A5-415F-848B-0A61A52C5C1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA11D56-76F8-49C1-91D6-88B61F5535C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7149" windowHeight="2614" xr2:uid="{BBF5B598-23F2-4CAF-8950-11568DE92F9C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>Graph 01        5</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>exact</t>
+  </si>
+  <si>
+    <t>iso nodes</t>
+  </si>
+  <si>
+    <t>cut verts</t>
   </si>
 </sst>
 </file>
@@ -585,283 +591,529 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79E6403-583E-4F38-A99A-D9FFC217D789}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="29.69140625" customWidth="1"/>
     <col min="2" max="2" width="6.15234375" customWidth="1"/>
-    <col min="5" max="5" width="9.4609375" customWidth="1"/>
-    <col min="6" max="6" width="2.4609375" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="9.84375" customWidth="1"/>
-    <col min="10" max="10" width="2.3828125" customWidth="1"/>
-    <col min="13" max="13" width="10.921875" customWidth="1"/>
-    <col min="14" max="14" width="2.53515625" customWidth="1"/>
+    <col min="6" max="6" width="9.4609375" customWidth="1"/>
+    <col min="7" max="7" width="2.4609375" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="9.84375" customWidth="1"/>
+    <col min="11" max="11" width="2.3828125" customWidth="1"/>
+    <col min="14" max="14" width="10.921875" customWidth="1"/>
+    <col min="15" max="15" width="2.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>48</v>
       </c>
       <c r="C1" t="s">
         <v>49</v>
       </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
       <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>46</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>68</v>
+      </c>
+      <c r="C2">
+        <v>408</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>6</v>
       </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="H2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="B3">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <v>183</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
         <v>10</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2">
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>447</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="B5">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <v>302</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2">
         <v>11</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2">
+      <c r="B6">
+        <v>51</v>
+      </c>
+      <c r="C6">
+        <v>51</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2">
         <v>4</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="B7">
+        <v>866</v>
+      </c>
+      <c r="C7">
+        <v>18710</v>
+      </c>
+      <c r="D7">
+        <v>343</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2">
         <v>54</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>81</v>
+      </c>
+      <c r="C8">
+        <v>810</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>8</v>
       </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="H8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="2">
+      <c r="B9">
+        <v>92</v>
+      </c>
+      <c r="C9">
+        <v>91</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>22</v>
+      </c>
+      <c r="F9" s="2">
         <v>2</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="2">
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>384</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
         <v>16</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <v>204</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
       <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>6</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="B12">
+        <v>60</v>
+      </c>
+      <c r="C12">
+        <v>1389</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
       <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
         <v>22</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B13">
+        <v>208</v>
+      </c>
+      <c r="C13">
+        <v>208</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
       <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
         <v>7</v>
       </c>
-      <c r="G13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="H13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="2">
+      <c r="B14">
         <v>31</v>
       </c>
-      <c r="G14">
+      <c r="C14">
+        <v>465</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>31</v>
+      </c>
+      <c r="H14">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B15">
+        <v>80</v>
+      </c>
+      <c r="C15">
+        <v>292</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
       <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
         <v>5</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B16">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>45</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
       <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
         <v>5</v>
       </c>
-      <c r="G16" s="5">
-        <v>3</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="H16" s="5">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B17">
+        <v>55</v>
+      </c>
+      <c r="C17">
+        <v>482</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
       <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
         <v>10</v>
       </c>
-      <c r="G17" s="4">
+      <c r="H17" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="2">
-        <v>3</v>
-      </c>
-      <c r="G18" s="5">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3</v>
+      </c>
+      <c r="H18" s="5">
         <v>2</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="2">
+      <c r="B19">
+        <v>194</v>
+      </c>
+      <c r="C19">
+        <v>2364</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
         <v>8</v>
       </c>
-      <c r="G19" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="H19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="2">
+      <c r="B20">
+        <v>190</v>
+      </c>
+      <c r="C20">
+        <v>3887</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
         <v>31</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="2">
+      <c r="B21">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>126</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
         <v>4</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -871,21 +1123,27 @@
       <c r="C23">
         <v>252</v>
       </c>
-      <c r="E23" s="2">
-        <v>3</v>
-      </c>
-      <c r="G23" s="2">
-        <v>3</v>
-      </c>
-      <c r="I23" t="s">
-        <v>42</v>
-      </c>
-      <c r="K23">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" s="2">
+        <v>3</v>
+      </c>
+      <c r="H23" s="2">
+        <v>3</v>
+      </c>
+      <c r="J23" t="s">
+        <v>42</v>
+      </c>
+      <c r="L23">
         <f>(SUMSQ(B23)/(SUMSQ(B23)-2*C23))</f>
         <v>1.0113411341134113</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -895,21 +1153,27 @@
       <c r="C24">
         <v>1028</v>
       </c>
-      <c r="E24" s="3">
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>23</v>
+      </c>
+      <c r="F24" s="3">
         <v>4</v>
       </c>
-      <c r="G24">
-        <v>3</v>
-      </c>
-      <c r="I24" t="s">
-        <v>42</v>
-      </c>
-      <c r="K24">
-        <f t="shared" ref="K24:K42" si="0">(SUMSQ(B24)/(SUMSQ(B24)-2*C24))</f>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="J24" t="s">
+        <v>42</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ref="L24:L42" si="0">(SUMSQ(B24)/(SUMSQ(B24)-2*C24))</f>
         <v>1.0099863998445697</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -919,21 +1183,27 @@
       <c r="C25">
         <v>1267</v>
       </c>
-      <c r="E25" s="3">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25" s="3">
         <v>7</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>4</v>
       </c>
-      <c r="I25" t="s">
-        <v>42</v>
-      </c>
-      <c r="K25">
+      <c r="J25" t="s">
+        <v>42</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="0"/>
         <v>1.0563236274727716</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -943,21 +1213,27 @@
       <c r="C26">
         <v>516</v>
       </c>
-      <c r="E26" s="3">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26" s="3">
         <v>5</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>4</v>
       </c>
-      <c r="I26" t="s">
-        <v>42</v>
-      </c>
-      <c r="K26">
+      <c r="J26" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26">
         <f t="shared" si="0"/>
         <v>1.0990688297974465</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -967,21 +1243,27 @@
       <c r="C27">
         <v>1198933</v>
       </c>
-      <c r="E27" s="2">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27" s="2">
         <v>2</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>2</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <f t="shared" si="0"/>
         <v>1.1755625913051539</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -991,21 +1273,27 @@
       <c r="C28">
         <v>271</v>
       </c>
-      <c r="E28" s="2">
-        <v>3</v>
-      </c>
-      <c r="G28" s="2">
-        <v>3</v>
-      </c>
-      <c r="I28" t="s">
-        <v>42</v>
-      </c>
-      <c r="K28">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>516</v>
+      </c>
+      <c r="F28" s="2">
+        <v>3</v>
+      </c>
+      <c r="H28" s="2">
+        <v>3</v>
+      </c>
+      <c r="J28" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28">
         <f t="shared" si="0"/>
         <v>1.0019405726479507</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -1015,21 +1303,27 @@
       <c r="C29">
         <v>529</v>
       </c>
-      <c r="E29" s="3">
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29" s="3">
         <v>12</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>8</v>
       </c>
-      <c r="I29" t="s">
-        <v>42</v>
-      </c>
-      <c r="K29">
+      <c r="J29" t="s">
+        <v>42</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="0"/>
         <v>2.3375474083438683</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1039,21 +1333,27 @@
       <c r="C30">
         <v>4955</v>
       </c>
-      <c r="E30" s="3">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>6</v>
+      </c>
+      <c r="F30" s="3">
         <v>98</v>
       </c>
-      <c r="G30" s="7">
+      <c r="H30" s="7">
         <v>6</v>
       </c>
-      <c r="I30" t="s">
-        <v>42</v>
-      </c>
-      <c r="K30" s="6">
+      <c r="J30" t="s">
+        <v>42</v>
+      </c>
+      <c r="L30" s="6">
         <f t="shared" si="0"/>
         <v>7.4392462638076671</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1063,21 +1363,27 @@
       <c r="C31">
         <v>961</v>
       </c>
-      <c r="E31" s="3">
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31" s="3">
         <v>5</v>
       </c>
-      <c r="G31">
-        <v>3</v>
-      </c>
-      <c r="I31" t="s">
-        <v>42</v>
-      </c>
-      <c r="K31">
+      <c r="H31">
+        <v>3</v>
+      </c>
+      <c r="J31" t="s">
+        <v>42</v>
+      </c>
+      <c r="L31">
         <f t="shared" si="0"/>
         <v>1.0474403909759589</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -1087,21 +1393,27 @@
       <c r="C32">
         <v>197</v>
       </c>
-      <c r="E32" s="2">
-        <v>3</v>
-      </c>
-      <c r="G32" s="2">
-        <v>3</v>
-      </c>
-      <c r="I32" t="s">
-        <v>42</v>
-      </c>
-      <c r="K32">
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>6</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3</v>
+      </c>
+      <c r="H32" s="2">
+        <v>3</v>
+      </c>
+      <c r="J32" t="s">
+        <v>42</v>
+      </c>
+      <c r="L32">
         <f t="shared" si="0"/>
         <v>1.0145055592371697</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1111,21 +1423,27 @@
       <c r="C33">
         <v>889</v>
       </c>
-      <c r="E33" s="3">
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33" s="3">
         <v>15</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>5</v>
       </c>
-      <c r="I33" t="s">
-        <v>42</v>
-      </c>
-      <c r="K33">
+      <c r="J33" t="s">
+        <v>42</v>
+      </c>
+      <c r="L33">
         <f t="shared" si="0"/>
         <v>1.070785890596385</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1135,21 +1453,27 @@
       <c r="C34">
         <v>744</v>
       </c>
-      <c r="E34" s="2">
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>173</v>
+      </c>
+      <c r="F34" s="2">
         <v>2</v>
       </c>
-      <c r="G34" s="2">
+      <c r="H34" s="2">
         <v>2</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <f t="shared" si="0"/>
         <v>1.0026954177897573</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -1159,24 +1483,30 @@
       <c r="C35">
         <v>1060</v>
       </c>
-      <c r="E35" s="3">
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35" s="3">
         <v>13</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>7</v>
       </c>
-      <c r="I35" t="s">
-        <v>42</v>
-      </c>
-      <c r="K35">
+      <c r="J35" t="s">
+        <v>42</v>
+      </c>
+      <c r="L35">
         <f t="shared" si="0"/>
         <v>1.4152791380999021</v>
       </c>
-      <c r="M35">
+      <c r="N35">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -1186,21 +1516,27 @@
       <c r="C36">
         <v>1808</v>
       </c>
-      <c r="E36" s="3">
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36" s="3">
         <v>4</v>
       </c>
-      <c r="G36">
-        <v>3</v>
-      </c>
-      <c r="I36" t="s">
-        <v>42</v>
-      </c>
-      <c r="K36">
+      <c r="H36">
+        <v>3</v>
+      </c>
+      <c r="J36" t="s">
+        <v>42</v>
+      </c>
+      <c r="L36">
         <f t="shared" si="0"/>
         <v>1.0044149625228775</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -1210,21 +1546,27 @@
       <c r="C37">
         <v>1642</v>
       </c>
-      <c r="E37" s="3">
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37" s="3">
         <v>9</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>5</v>
       </c>
-      <c r="I37" t="s">
-        <v>42</v>
-      </c>
-      <c r="K37">
+      <c r="J37" t="s">
+        <v>42</v>
+      </c>
+      <c r="L37">
         <f t="shared" si="0"/>
         <v>1.0764770266179176</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -1234,21 +1576,27 @@
       <c r="C38">
         <v>323</v>
       </c>
-      <c r="E38" s="3">
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38" s="3">
         <v>4</v>
       </c>
-      <c r="G38">
-        <v>3</v>
-      </c>
-      <c r="I38" t="s">
-        <v>42</v>
-      </c>
-      <c r="K38">
+      <c r="H38">
+        <v>3</v>
+      </c>
+      <c r="J38" t="s">
+        <v>42</v>
+      </c>
+      <c r="L38">
         <f t="shared" si="0"/>
         <v>1.0246095238095239</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -1258,21 +1606,27 @@
       <c r="C39">
         <v>96</v>
       </c>
-      <c r="E39" s="3">
+      <c r="D39">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>22</v>
+      </c>
+      <c r="F39" s="3">
         <v>8</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>6</v>
       </c>
-      <c r="I39" t="s">
-        <v>42</v>
-      </c>
-      <c r="K39">
+      <c r="J39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L39">
         <f t="shared" si="0"/>
         <v>1.0173850054328142</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -1282,21 +1636,27 @@
       <c r="C40">
         <v>1116</v>
       </c>
-      <c r="E40" s="3">
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40" s="3">
         <v>10</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>6</v>
       </c>
-      <c r="I40" t="s">
-        <v>42</v>
-      </c>
-      <c r="K40">
+      <c r="J40" t="s">
+        <v>42</v>
+      </c>
+      <c r="L40">
         <f t="shared" si="0"/>
         <v>1.1495076696362785</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
@@ -1306,21 +1666,27 @@
       <c r="C41">
         <v>498</v>
       </c>
-      <c r="E41" s="3">
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>25</v>
+      </c>
+      <c r="F41" s="3">
         <v>11</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>6</v>
       </c>
-      <c r="I41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K41">
+      <c r="J41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L41">
         <f t="shared" si="0"/>
         <v>1.051200328998098</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
@@ -1330,16 +1696,22 @@
       <c r="C42">
         <v>2502</v>
       </c>
-      <c r="E42" s="3">
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+      <c r="F42" s="3">
         <v>9</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>5</v>
       </c>
-      <c r="I42" t="s">
-        <v>42</v>
-      </c>
-      <c r="K42">
+      <c r="J42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L42">
         <f t="shared" si="0"/>
         <v>1.0345663661796705</v>
       </c>

</xml_diff>

<commit_message>
program ready for tournament
</commit_message>
<xml_diff>
--- a/someResults.xlsx
+++ b/someResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alain\Desktop\project1-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA11D56-76F8-49C1-91D6-88B61F5535C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3250EE2-083A-4A10-AF7E-2A12CD0FDD65}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7149" windowHeight="2614" xr2:uid="{BBF5B598-23F2-4CAF-8950-11568DE92F9C}"/>
   </bookViews>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79E6403-583E-4F38-A99A-D9FFC217D789}">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -990,7 +990,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1012,8 +1012,11 @@
       <c r="H17" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="N17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1108,12 +1111,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>1.0113411341134113</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>1.0099863998445697</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>1.0563236274727716</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>1.0990688297974465</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1263,7 +1266,7 @@
         <v>1.1755625913051539</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>1.0019405726479507</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -1323,7 +1326,7 @@
         <v>2.3375474083438683</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>7.4392462638076671</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1383,7 +1386,7 @@
         <v>1.0474403909759589</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>